<commit_message>
Updated the models for all competitions
</commit_message>
<xml_diff>
--- a/data/model_params_AFCON_2023.xlsx
+++ b/data/model_params_AFCON_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8180627407542272</v>
+        <v>0.1914962479904777</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.1204659403566293</v>
+        <v>-0.1142643096335048</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1501277895938733</v>
+        <v>-0.1475071333334574</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2507775802838664</v>
+        <v>-0.2231475834934862</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.4049510687217718</v>
+        <v>-0.4342047056573254</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.132419210039306</v>
+        <v>0.1232856110648965</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.255799451091021</v>
+        <v>0.255648357988816</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.00245024230745782</v>
+        <v>0.001991875202858949</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.07823676720304414</v>
+        <v>0.0646952354760759</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.268631351397555</v>
+        <v>0.8732820434956737</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.2166536936959607</v>
+        <v>0.8384664120137821</v>
       </c>
     </row>
     <row r="13">
@@ -562,17 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.6490988451563211</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>shot_during_regular_play</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>-1.062473816845795</v>
+        <v>-0.03003781585575057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>